<commit_message>
Implementing the new data example
</commit_message>
<xml_diff>
--- a/plotVars.xlsx
+++ b/plotVars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/PMX/Projects/Pharmetheus/PMXForest/PMXForest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C2AB47C-09B7-4744-BF29-7E78E7AD5432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03532083-79AB-CC48-90E8-13304E05F2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21720" yWindow="2980" windowWidth="28040" windowHeight="17440" xr2:uid="{3ED54772-DDF7-D844-9E8C-B2FD6B3902D1}"/>
+    <workbookView xWindow="33260" yWindow="7540" windowWidth="28040" windowHeight="17440" xr2:uid="{3ED54772-DDF7-D844-9E8C-B2FD6B3902D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
     <t>func</t>
   </si>
   <si>
-    <t>final</t>
-  </si>
-  <si>
     <t>point</t>
   </si>
   <si>
@@ -113,14 +110,25 @@
   </si>
   <si>
     <t>Q2_REL_REFTRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -148,8 +156,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,7 +476,7 @@
   <dimension ref="C3:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:I12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,13 +498,13 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>7</v>
       </c>
       <c r="I3" t="s">
         <v>2</v>
@@ -512,16 +521,16 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.2">
@@ -532,19 +541,19 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.2">
@@ -558,7 +567,7 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.2">
@@ -569,10 +578,10 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.2">
@@ -586,13 +595,13 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -606,18 +615,18 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <v>1</v>
       </c>
     </row>
@@ -632,13 +641,13 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
         <v>20</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>21</v>
-      </c>
-      <c r="H10" t="s">
-        <v>22</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -652,16 +661,16 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
         <v>23</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>24</v>
-      </c>
-      <c r="H11" t="s">
-        <v>25</v>
       </c>
       <c r="I11">
         <v>1</v>

</xml_diff>